<commit_message>
Fix misspelling of interruptible
</commit_message>
<xml_diff>
--- a/test_data/operations/control_requirements.xlsx
+++ b/test_data/operations/control_requirements.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtopper\Programming\Python\git\dtocean-core\test_data\operations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Python\git\dtocean-core\test_data\operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871DD12C-1762-4CBB-85C8-89D75084739C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="110" windowWidth="22980" windowHeight="8940" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="22980" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="On-Site" sheetId="1" r:id="rId1"/>
     <sheet name="Replacement" sheetId="2" r:id="rId2"/>
     <sheet name="Inspections" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
   <si>
     <t>False</t>
   </si>
@@ -63,12 +64,15 @@
   </si>
   <si>
     <t>Max Current Velocity</t>
+  </si>
+  <si>
+    <t>Interruptible</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -169,11 +173,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Explanatory Text 2" xfId="2"/>
+    <cellStyle name="Explanatory Text 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="4"/>
-    <cellStyle name="Normal 4" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 4" xfId="1" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -264,6 +268,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -299,6 +320,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -474,29 +512,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" customWidth="1"/>
-    <col min="4" max="4" width="20.81640625" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" customWidth="1"/>
-    <col min="6" max="6" width="26.26953125" customWidth="1"/>
-    <col min="7" max="7" width="18.6328125" customWidth="1"/>
-    <col min="8" max="8" width="17.54296875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
     <col min="9" max="10" width="7" customWidth="1"/>
-    <col min="11" max="11" width="16.54296875" customWidth="1"/>
-    <col min="12" max="12" width="18.6328125" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -534,7 +572,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -572,7 +610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -586,7 +624,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -595,7 +633,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -610,29 +648,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:L2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="30.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -640,7 +678,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>4</v>
@@ -658,7 +696,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -694,27 +732,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" customWidth="1"/>
-    <col min="3" max="3" width="20.81640625" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" customWidth="1"/>
-    <col min="5" max="5" width="18.6328125" customWidth="1"/>
-    <col min="6" max="6" width="17.54296875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
     <col min="7" max="8" width="7" customWidth="1"/>
-    <col min="9" max="9" width="16.54296875" customWidth="1"/>
-    <col min="10" max="10" width="18.6328125" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -746,7 +784,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Misspelling or iturruptible in tests
</commit_message>
<xml_diff>
--- a/test_data/operations/control_requirements.xlsx
+++ b/test_data/operations/control_requirements.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Python\git\dtocean-core\test_data\operations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871DD12C-1762-4CBB-85C8-89D75084739C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62417492-6DE1-4C1C-81C6-BCD6BDD529BC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="22980" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="22980" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="On-Site" sheetId="1" r:id="rId1"/>
     <sheet name="Replacement" sheetId="2" r:id="rId2"/>
     <sheet name="Inspections" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
   <si>
     <t>False</t>
   </si>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>Sub-System</t>
-  </si>
-  <si>
-    <t>Interruptable</t>
   </si>
   <si>
     <t>Crew Preparation Delay</t>
@@ -515,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,37 +536,37 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -651,7 +648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -675,25 +672,25 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -757,31 +754,31 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>